<commit_message>
1.3.5 inserção coluna preço médio
</commit_message>
<xml_diff>
--- a/dados_realiz-2023_tratados.xlsx
+++ b/dados_realiz-2023_tratados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,11 @@
           <t>Total Anual</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Preço Médio Pago</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -558,6 +563,9 @@
       <c r="O2" t="n">
         <v>4887.88</v>
       </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -607,6 +615,9 @@
       <c r="O3" t="n">
         <v>3070.99</v>
       </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -656,6 +667,9 @@
       <c r="O4" t="n">
         <v>2598</v>
       </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -705,6 +719,9 @@
       <c r="O5" t="n">
         <v>472.99</v>
       </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -752,7 +769,10 @@
         <v>226.25</v>
       </c>
       <c r="O6" t="n">
-        <v>1357.51</v>
+        <v>1562.71</v>
+      </c>
+      <c r="P6" t="n">
+        <v>205.2</v>
       </c>
     </row>
     <row r="7">
@@ -801,7 +821,10 @@
         <v>3.97</v>
       </c>
       <c r="O7" t="n">
-        <v>23.8</v>
+        <v>3375.4</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3351.6</v>
       </c>
     </row>
     <row r="8">
@@ -850,7 +873,10 @@
         <v>25.45</v>
       </c>
       <c r="O8" t="n">
-        <v>152.7</v>
+        <v>3379.84</v>
+      </c>
+      <c r="P8" t="n">
+        <v>3227.14</v>
       </c>
     </row>
     <row r="9">
@@ -899,7 +925,10 @@
         <v>46.45</v>
       </c>
       <c r="O9" t="n">
-        <v>278.69</v>
+        <v>3498.13</v>
+      </c>
+      <c r="P9" t="n">
+        <v>3219.44</v>
       </c>
     </row>
     <row r="10">
@@ -948,7 +977,10 @@
         <v>44.8</v>
       </c>
       <c r="O10" t="n">
-        <v>268.82</v>
+        <v>3264.12</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2995.3</v>
       </c>
     </row>
     <row r="11">
@@ -997,7 +1029,10 @@
         <v>33.5</v>
       </c>
       <c r="O11" t="n">
-        <v>201</v>
+        <v>3244.3</v>
+      </c>
+      <c r="P11" t="n">
+        <v>3043.3</v>
       </c>
     </row>
     <row r="12">
@@ -1046,7 +1081,10 @@
         <v>29.33</v>
       </c>
       <c r="O12" t="n">
-        <v>176</v>
+        <v>3218.39</v>
+      </c>
+      <c r="P12" t="n">
+        <v>3042.39</v>
       </c>
     </row>
     <row r="13">
@@ -1095,7 +1133,10 @@
         <v>21.67</v>
       </c>
       <c r="O13" t="n">
-        <v>130</v>
+        <v>3148.54</v>
+      </c>
+      <c r="P13" t="n">
+        <v>3018.54</v>
       </c>
     </row>
     <row r="14">
@@ -1146,6 +1187,9 @@
       <c r="O14" t="n">
         <v>126.5</v>
       </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1195,6 +1239,9 @@
       <c r="O15" t="n">
         <v>459.38</v>
       </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1244,6 +1291,9 @@
       <c r="O16" t="n">
         <v>38.79</v>
       </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1293,6 +1343,9 @@
       <c r="O17" t="n">
         <v>107.97</v>
       </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1342,6 +1395,9 @@
       <c r="O18" t="n">
         <v>101.78</v>
       </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1391,6 +1447,9 @@
       <c r="O19" t="n">
         <v>148.31</v>
       </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1440,6 +1499,9 @@
       <c r="O20" t="n">
         <v>62.53</v>
       </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1489,6 +1551,9 @@
       <c r="O21" t="n">
         <v>0</v>
       </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1536,6 +1601,9 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.3.6 inserção linha vsho11
</commit_message>
<xml_diff>
--- a/dados_realiz-2023_tratados.xlsx
+++ b/dados_realiz-2023_tratados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e62e7c97e835051/Altieri/Softwares/Dev/Projetos Pessoais/Projeto_Carteira_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_4DF5D3B2D300D562177B2211595ED87656CD0F7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED512DD-49E9-42BC-90F9-AFE637623347}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_4DF5D3B2D300D562177B2211595ED87656CD0F7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{238BF67F-5B7F-40C8-9E88-29FA326C065D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,6 +206,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,7 +500,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,13 +563,13 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="E2">
         <v>462.97</v>
@@ -709,13 +713,13 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>150</v>

</xml_diff>